<commit_message>
Replace sort from drinks
</commit_message>
<xml_diff>
--- a/wine3.xlsx
+++ b/wine3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Илья\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pythonchik\!devman progs\projects\wine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1B18A6-D0D5-46C6-8795-EDD6EAD4D101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE610BC-77EF-4781-AAC0-568152AC5BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -64,52 +64,52 @@
     <t>Белые вина</t>
   </si>
   <si>
+    <t>Коньяк классический</t>
+  </si>
+  <si>
+    <t>konyak_klassicheskyi.png</t>
+  </si>
+  <si>
+    <t>Красные вина</t>
+  </si>
+  <si>
+    <t>Черный лекарь</t>
+  </si>
+  <si>
+    <t>Качич</t>
+  </si>
+  <si>
+    <t>chernyi_lekar.png</t>
+  </si>
+  <si>
+    <t>Кокур</t>
+  </si>
+  <si>
+    <t>kokur.png</t>
+  </si>
+  <si>
+    <t>Киндзмараули</t>
+  </si>
+  <si>
+    <t>Саперави</t>
+  </si>
+  <si>
+    <t>kindzmarauli.png</t>
+  </si>
+  <si>
+    <t>Чача</t>
+  </si>
+  <si>
+    <t>chacha.png</t>
+  </si>
+  <si>
+    <t>Коньяк кизиловый</t>
+  </si>
+  <si>
+    <t>konyak_kizilovyi.png</t>
+  </si>
+  <si>
     <t>Напитки</t>
-  </si>
-  <si>
-    <t>Коньяк классический</t>
-  </si>
-  <si>
-    <t>konyak_klassicheskyi.png</t>
-  </si>
-  <si>
-    <t>Красные вина</t>
-  </si>
-  <si>
-    <t>Черный лекарь</t>
-  </si>
-  <si>
-    <t>Качич</t>
-  </si>
-  <si>
-    <t>chernyi_lekar.png</t>
-  </si>
-  <si>
-    <t>Кокур</t>
-  </si>
-  <si>
-    <t>kokur.png</t>
-  </si>
-  <si>
-    <t>Киндзмараули</t>
-  </si>
-  <si>
-    <t>Саперави</t>
-  </si>
-  <si>
-    <t>kindzmarauli.png</t>
-  </si>
-  <si>
-    <t>Чача</t>
-  </si>
-  <si>
-    <t>chacha.png</t>
-  </si>
-  <si>
-    <t>Коньяк кизиловый</t>
-  </si>
-  <si>
-    <t>konyak_kizilovyi.png</t>
   </si>
 </sst>
 </file>
@@ -399,19 +399,19 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -428,7 +428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -445,22 +445,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3">
         <v>350</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -477,26 +477,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="D5" s="3">
         <v>399</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
@@ -511,68 +511,68 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3">
         <v>450</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D8" s="3">
         <v>550</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3">
         <v>299</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3">
         <v>350</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>